<commit_message>
Working - Needs Exception Handling
Many changes involved in editing vs creating users.
</commit_message>
<xml_diff>
--- a/New_Apex_Users.xlsx
+++ b/New_Apex_Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tmgolf-my.sharepoint.com/personal/brandon_yates_taylormadegolf_com/Documents/Documents/GitHub/Apex-Revamped/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1953" documentId="13_ncr:1_{8E09E700-47DA-4F61-8A8F-DCB1AD3AABF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52872F15-E693-465B-A419-5779D276B3DC}"/>
+  <xr:revisionPtr revIDLastSave="1978" documentId="13_ncr:1_{8E09E700-47DA-4F61-8A8F-DCB1AD3AABF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65296F35-4234-4815-A0E1-4A76D1591083}"/>
   <bookViews>
     <workbookView xWindow="-21315" yWindow="825" windowWidth="17250" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="664">
   <si>
     <t>First Name</t>
   </si>
@@ -1989,13 +1989,46 @@
     <t>Paulis</t>
   </si>
   <si>
-    <t xml:space="preserve">Python </t>
-  </si>
-  <si>
-    <t>Test</t>
+    <t>Python</t>
   </si>
   <si>
     <t>General</t>
+  </si>
+  <si>
+    <t>Bot 1</t>
+  </si>
+  <si>
+    <t>Bot 2</t>
+  </si>
+  <si>
+    <t>Bot 3</t>
+  </si>
+  <si>
+    <t>Bot 4</t>
+  </si>
+  <si>
+    <t>Bot 5</t>
+  </si>
+  <si>
+    <t>Bot 6</t>
+  </si>
+  <si>
+    <t>Bot 7</t>
+  </si>
+  <si>
+    <t>Bot 8</t>
+  </si>
+  <si>
+    <t>Bot 9</t>
+  </si>
+  <si>
+    <t>Bot 10</t>
+  </si>
+  <si>
+    <t>Bot 11</t>
+  </si>
+  <si>
+    <t>Bot 12</t>
   </si>
 </sst>
 </file>
@@ -2619,7 +2652,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2656,13 +2689,13 @@
         <v>650</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C2" s="8">
-        <v>11113</v>
+        <v>11125</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -2673,13 +2706,13 @@
         <v>650</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="C3" s="8">
+        <v>11126</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>651</v>
-      </c>
-      <c r="C3" s="8">
-        <v>4444</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -2690,10 +2723,10 @@
         <v>650</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="C4" s="8">
-        <v>11115</v>
+        <v>11127</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>7</v>
@@ -2707,13 +2740,13 @@
         <v>650</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="C5" s="8">
-        <v>6666</v>
+        <v>11128</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2721,13 +2754,13 @@
         <v>650</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>651</v>
+        <v>656</v>
       </c>
       <c r="C6" s="8">
-        <v>11117</v>
+        <v>11129</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2735,13 +2768,13 @@
         <v>650</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>651</v>
+        <v>657</v>
       </c>
       <c r="C7" s="8">
-        <v>11118</v>
+        <v>11130</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2749,13 +2782,13 @@
         <v>650</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="C8" s="8">
+        <v>11131</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>651</v>
-      </c>
-      <c r="C8" s="8">
-        <v>11119</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2763,13 +2796,13 @@
         <v>650</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>651</v>
+        <v>659</v>
       </c>
       <c r="C9" s="8">
-        <v>11120</v>
+        <v>11132</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>652</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2777,10 +2810,10 @@
         <v>650</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>651</v>
+        <v>660</v>
       </c>
       <c r="C10" s="8">
-        <v>11121</v>
+        <v>11133</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>10</v>
@@ -2791,10 +2824,10 @@
         <v>650</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>651</v>
+        <v>661</v>
       </c>
       <c r="C11" s="8">
-        <v>11122</v>
+        <v>11134</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>16</v>
@@ -2805,10 +2838,10 @@
         <v>650</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>651</v>
+        <v>662</v>
       </c>
       <c r="C12" s="8">
-        <v>11123</v>
+        <v>11135</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>13</v>
@@ -2819,13 +2852,13 @@
         <v>650</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
       <c r="C13" s="8">
-        <v>11124</v>
+        <v>11136</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -10190,6 +10223,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC7C19C8B79DF846A59EF11074BAA4E6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac75452dfaff1ddbee136b983182fa5f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="64f8f827-b2a5-48dc-b2c3-f16a6c19a3e1" xmlns:ns3="19fc8c01-1281-4c4f-a9d6-4eaecf49cf8c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b0f6662259a420d4235d7fe97ace352" ns2:_="" ns3:_="">
     <xsd:import namespace="64f8f827-b2a5-48dc-b2c3-f16a6c19a3e1"/>
@@ -10406,15 +10448,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{516C47DE-5E69-4ED4-B335-2D06DB8F4F74}">
   <ds:schemaRefs>
@@ -10427,6 +10460,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31236C6E-5FF1-4D70-876A-B16E5BFCC253}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8608753D-D904-4E13-B351-DF9ECED19E3C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10443,12 +10484,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31236C6E-5FF1-4D70-876A-B16E5BFCC253}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>